<commit_message>
changed setpoints to not overlap
</commit_message>
<xml_diff>
--- a/projects/office_calibration_14.xlsx
+++ b/projects/office_calibration_14.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="13176" tabRatio="562" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="13176" tabRatio="562" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -6875,7 +6875,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -7343,9 +7343,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y224"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A106" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A102" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N106" sqref="N106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9856,20 +9856,20 @@
       </c>
       <c r="I106" s="46"/>
       <c r="J106" s="45">
-        <v>-5</v>
+        <v>-2</v>
       </c>
       <c r="K106" s="45">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="L106" s="45">
         <v>0</v>
       </c>
       <c r="M106" s="45">
         <f>(K106-J106)/6</f>
-        <v>1.6666666666666667</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="N106" s="45">
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="Q106" s="43" t="s">
         <v>776</v>
@@ -9896,20 +9896,20 @@
       </c>
       <c r="I107" s="46"/>
       <c r="J107" s="45">
-        <v>-5</v>
+        <v>-2</v>
       </c>
       <c r="K107" s="45">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="L107" s="45">
         <v>0</v>
       </c>
       <c r="M107" s="45">
         <f>(K107-J107)/6</f>
-        <v>1.6666666666666667</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="N107" s="45">
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="Q107" s="43" t="s">
         <v>776</v>

</xml_diff>